<commit_message>
added an exception for get pages num
</commit_message>
<xml_diff>
--- a/downloads/sephora_data.xlsx
+++ b/downloads/sephora_data.xlsx
@@ -37,12 +37,12 @@
     <t>Almost Lipstick</t>
   </si>
   <si>
+    <t>Moisture Surge 100H Auto-Replenishing Hydrator Moisturizer</t>
+  </si>
+  <si>
     <t>High Impact Mascara</t>
   </si>
   <si>
-    <t>Moisture Surge 100H Auto-Replenishing Hydrator Moisturizer</t>
-  </si>
-  <si>
     <t>Take The Day Off Cleansing Balm Makeup Remover</t>
   </si>
   <si>
@@ -61,22 +61,25 @@
     <t>Cheek Pop Blush</t>
   </si>
   <si>
+    <t>Even Better Makeup Broad Spectrum SPF 15 Foundation</t>
+  </si>
+  <si>
     <t>Stay-Matte Sheer Pressed Powder</t>
   </si>
   <si>
-    <t>Even Better Makeup Broad Spectrum SPF 15 Foundation</t>
+    <t>All About Shadow 8-Pan Palette</t>
+  </si>
+  <si>
+    <t>Dramatically Different Moisturizing Gel</t>
+  </si>
+  <si>
+    <t>All About Eyes Eye Cream with Vitamin C</t>
   </si>
   <si>
     <t>All About Clean Liquid Facial Soap</t>
   </si>
   <si>
-    <t>Dramatically Different Moisturizing Gel</t>
-  </si>
-  <si>
-    <t>All About Shadow 8-Pan Palette</t>
-  </si>
-  <si>
-    <t>All About Eyes Eye Cream with Vitamin C</t>
+    <t>High Impact High-Fi Full Volume Mascara</t>
   </si>
   <si>
     <t>Clarifying Lotion 2</t>
@@ -91,7 +94,7 @@
     <t>Beyond Perfecting Foundation + Concealer</t>
   </si>
   <si>
-    <t>High Impact High-Fi Full Volume Mascara</t>
+    <t>Acne Solutions Clarifying Lotion</t>
   </si>
   <si>
     <t>Clarifying Lotion 3</t>
@@ -100,27 +103,27 @@
     <t>Take The Day Off Micellar Cleansing Towelettes for Face &amp; Eyes Makeup Remover</t>
   </si>
   <si>
-    <t>Acne Solutions Clarifying Lotion</t>
-  </si>
-  <si>
     <t>Moisture Surge CC Cream Hydrating Colour Corrector Broad Spectrum SPF 30</t>
   </si>
   <si>
+    <t>All About Eyes Serum De-Puffing Eye Massage</t>
+  </si>
+  <si>
     <t>Moisture Surge Broad Spectrum Sunscreen SPF 28 Sheer Hydrator Moisturizer</t>
   </si>
   <si>
+    <t>Rinse-Off Foaming Cleanser</t>
+  </si>
+  <si>
+    <t>Even Better Clinical Radical Dark Spot Corrector + Interrupter Serum</t>
+  </si>
+  <si>
+    <t>Even Better Clinical Serum Foundation Broad Spectrum SPF 25</t>
+  </si>
+  <si>
     <t>Mini Take The Day Off Cleansing Balm Makeup Remover</t>
   </si>
   <si>
-    <t>Rinse-Off Foaming Cleanser</t>
-  </si>
-  <si>
-    <t>Even Better Clinical Radical Dark Spot Corrector + Interrupter Serum</t>
-  </si>
-  <si>
-    <t>Even Better Clinical Serum Foundation Broad Spectrum SPF 25</t>
-  </si>
-  <si>
     <t>Acne Solutions Clinical Clearing Gel</t>
   </si>
   <si>
@@ -130,90 +133,99 @@
     <t>Moisture Surge Sheertint Hydrator Broad Spectrum SPF 25 Tinted Moisturizer</t>
   </si>
   <si>
-    <t>All About Eyes Serum De-Puffing Eye Massage</t>
+    <t>Quickliner&amp;trade; For Eyes Eyeliner</t>
+  </si>
+  <si>
+    <t>Exfoliating Face Scrub</t>
   </si>
   <si>
     <t>Take The Day Off Cleansing Oil Makeup Remover</t>
   </si>
   <si>
-    <t>Exfoliating Face Scrub</t>
+    <t>Moisture Surge Intense 72H Lipid-Replenishing Hydrator Moisturizer</t>
   </si>
   <si>
     <t>High Impact&amp;trade; Mascara Mini</t>
   </si>
   <si>
-    <t>Quickliner&amp;trade; For Eyes Eyeliner</t>
-  </si>
-  <si>
     <t>Smart Clinical Repair&amp;trade; Wrinkle Correcting Serum</t>
   </si>
   <si>
+    <t>Moisture Megastars Hydrating Skincare Set</t>
+  </si>
+  <si>
+    <t>All About Eyes Rich Eye Cream with Hyaluronic Acid</t>
+  </si>
+  <si>
+    <t>Smart Clinical Repair Wrinkle Correcting Cream</t>
+  </si>
+  <si>
+    <t>Mini Dramatically Different Moisturizing Gel</t>
+  </si>
+  <si>
     <t>High Impact Waterproof Mascara</t>
   </si>
   <si>
-    <t>Moisture Megastars Hydrating Skincare Set</t>
-  </si>
-  <si>
-    <t>Mini Dramatically Different Moisturizing Gel</t>
-  </si>
-  <si>
-    <t>Moisture Surge Intense 72H Lipid-Replenishing Hydrator Moisturizer</t>
-  </si>
-  <si>
     <t>Mini Take The Day Off Makeup Remover For Lids, Lashes &amp; Lips</t>
   </si>
   <si>
-    <t>Smart Clinical Repair Wrinkle Correcting Cream</t>
+    <t>All About Shadow&amp;trade; Single Eye Shadow</t>
+  </si>
+  <si>
+    <t>Acne Solutions All-Over Clearing Treatment Oil-Free</t>
   </si>
   <si>
     <t>Blended Face Powder</t>
   </si>
   <si>
-    <t>All About Eyes Rich Eye Cream with Hyaluronic Acid</t>
+    <t>Mini Dramatically Different Moisturizing Lotion+</t>
+  </si>
+  <si>
+    <t>Great Skin, Great Deal Set for Combination Oily Skin</t>
+  </si>
+  <si>
+    <t>Dramatically Different Hydrating Jelly</t>
+  </si>
+  <si>
+    <t>7 Day Face Scrub Cream Rinse-Off Formula</t>
+  </si>
+  <si>
+    <t>Mini Moisture Surge Broad Spectrum SPF 28 Sheer Hydrator Moisturizer</t>
   </si>
   <si>
     <t>Lash Building Primer</t>
   </si>
   <si>
-    <t>All About Shadow&amp;trade; Single Eye Shadow</t>
-  </si>
-  <si>
-    <t>Mini Dramatically Different Moisturizing Lotion+</t>
-  </si>
-  <si>
-    <t>Dramatically Different Hydrating Jelly</t>
-  </si>
-  <si>
-    <t>Mini Moisture Surge Broad Spectrum SPF 28 Sheer Hydrator Moisturizer</t>
-  </si>
-  <si>
-    <t>Great Skin, Great Deal Set for Combination Oily Skin</t>
-  </si>
-  <si>
     <t>Redness Solutions with Probiotic Technology Daily Relief Cream</t>
   </si>
   <si>
+    <t>High Impact Easy Liquid Eyeliner</t>
+  </si>
+  <si>
+    <t>Mini Moisture Surge 100H Auto-Replenishing Hydrator Moisturizer</t>
+  </si>
+  <si>
+    <t>High Impact Extreme Volume Mascara</t>
+  </si>
+  <si>
     <t>Smart Clinical Repair&amp;trade; Wrinkle Correcting Eye Cream</t>
   </si>
   <si>
-    <t>Acne Solutions All-Over Clearing Treatment Oil-Free</t>
-  </si>
-  <si>
-    <t>High Impact Easy Liquid Eyeliner</t>
-  </si>
-  <si>
-    <t>7 Day Face Scrub Cream Rinse-Off Formula</t>
-  </si>
-  <si>
-    <t>Mini Moisture Surge 100H Auto-Replenishing Hydrator Moisturizer</t>
-  </si>
-  <si>
-    <t>High Impact Extreme Volume Mascara</t>
+    <t>Acne Solutions Acne + Line Correcting Serum</t>
+  </si>
+  <si>
+    <t>Take The Day Off Facial Cleansing Mousse</t>
   </si>
   <si>
     <t>Moisture Surge Overnight Face Mask</t>
   </si>
   <si>
+    <t>Mineral Face Sunscreen Broad Spectrum SPF 50</t>
+  </si>
+  <si>
+    <t>Clinique For Men Anti-Age Moisturizer</t>
+  </si>
+  <si>
     <t>Moisture Surge Eye 96-Hour Hydro-Filler Concentrate</t>
   </si>
   <si>
@@ -223,9 +235,6 @@
     <t>Blackhead Solutions 7 Day Deep Pore Cleanse &amp; Face Scrub</t>
   </si>
   <si>
-    <t>Take The Day Off Facial Cleansing Mousse</t>
-  </si>
-  <si>
     <t>Moisture Surge Hydrating Supercharged Concentrate</t>
   </si>
   <si>
@@ -235,24 +244,18 @@
     <t>All About Clean&amp;trade; 2-in-1 Cleansing + Exfoliating Jelly</t>
   </si>
   <si>
+    <t>Blackhead Solutions Self-heating Blackhead Extractor</t>
+  </si>
+  <si>
+    <t>Mini Acne Solutions Clinical Clearing Gel</t>
+  </si>
+  <si>
+    <t>Face Sunscreen Broad Spectrum SPF 50</t>
+  </si>
+  <si>
     <t>Clarifying Lotion 1</t>
   </si>
   <si>
-    <t>Blackhead Solutions Self-heating Blackhead Extractor</t>
-  </si>
-  <si>
-    <t>Mini Acne Solutions Clinical Clearing Gel</t>
-  </si>
-  <si>
-    <t>Mineral Face Sunscreen Broad Spectrum SPF 50</t>
-  </si>
-  <si>
-    <t>Face Sunscreen Broad Spectrum SPF 50</t>
-  </si>
-  <si>
-    <t>Acne Solutions Acne + Line Correcting Serum</t>
-  </si>
-  <si>
     <t>Clarifying Lotion 4</t>
   </si>
   <si>
@@ -262,75 +265,81 @@
     <t>Superdefense City Block Face Sunscreen SPF 50</t>
   </si>
   <si>
+    <t>Redness Solutions Soothing Cleanser</t>
+  </si>
+  <si>
+    <t>Exfoliating Tonic</t>
+  </si>
+  <si>
+    <t>Age Defense BB Cream Broad Spectrum SPF 30</t>
+  </si>
+  <si>
+    <t>Clinique For Men&amp;trade; Anti-Age Eye Cream</t>
+  </si>
+  <si>
+    <t>Pop Splash&amp;trade; Lip Gloss</t>
+  </si>
+  <si>
+    <t>Even Better Brightening Moisturizer SPF 20</t>
+  </si>
+  <si>
+    <t>Mini Take The Day Off Charcoal Cleansing Balm Makeup Remover</t>
+  </si>
+  <si>
+    <t>City Block&amp;trade; Sheer Oil-Free Daily Face Protector Broad Spectrum Sunscreen SPF 25 Primer</t>
+  </si>
+  <si>
+    <t>True Bronze Pressed Powder Bronzer</t>
+  </si>
+  <si>
+    <t>Even Better Eyes Dark Circle Corrector</t>
+  </si>
+  <si>
+    <t>All About Clean 2-in-1 Charcoal Face Mask + Scrub</t>
+  </si>
+  <si>
     <t>Repairwear Anti-Gravity Eye Cream</t>
   </si>
   <si>
-    <t>Redness Solutions Soothing Cleanser</t>
-  </si>
-  <si>
-    <t>Exfoliating Tonic</t>
-  </si>
-  <si>
-    <t>Clinique For Men Anti-Age Moisturizer</t>
-  </si>
-  <si>
-    <t>Age Defense BB Cream Broad Spectrum SPF 30</t>
-  </si>
-  <si>
-    <t>Even Better Brightening Moisturizer SPF 20</t>
-  </si>
-  <si>
-    <t>Mini Take The Day Off Charcoal Cleansing Balm Makeup Remover</t>
-  </si>
-  <si>
-    <t>City Block&amp;trade; Sheer Oil-Free Daily Face Protector Broad Spectrum Sunscreen SPF 25 Primer</t>
-  </si>
-  <si>
-    <t>True Bronze Pressed Powder Bronzer</t>
-  </si>
-  <si>
-    <t>Pop Splash&amp;trade; Lip Gloss</t>
-  </si>
-  <si>
-    <t>Even Better Eyes Dark Circle Corrector</t>
-  </si>
-  <si>
-    <t>All About Clean 2-in-1 Charcoal Face Mask + Scrub</t>
-  </si>
-  <si>
     <t>Dramatically Different Moisturizing Cream</t>
   </si>
   <si>
+    <t>Broad Spectrum SPF 21 Moisturizer</t>
+  </si>
+  <si>
+    <t>Sparkle Skin Body Exfoliator</t>
+  </si>
+  <si>
+    <t>Clinique For Men Super Energizer&amp;trade; Anti-Fatigue Depuffing Eye Gel</t>
+  </si>
+  <si>
+    <t>Moisturizing Lotion</t>
+  </si>
+  <si>
+    <t>Face Scrub</t>
+  </si>
+  <si>
+    <t>Repairwear Laser Focus Wrinkle Correcting Eye Cream</t>
+  </si>
+  <si>
+    <t>Even Better Clinical Brightening Moisturizer</t>
+  </si>
+  <si>
+    <t>Clinique For Men Maximum Hydrator 72-Hour Auto-Replenishing Hydrator</t>
+  </si>
+  <si>
+    <t>Fresh Pressed Daily Booster with Pure Vitamin C 10%</t>
+  </si>
+  <si>
+    <t>Smart Clinical Repair Wrinkle Correcting Rich Cream</t>
+  </si>
+  <si>
     <t>Charcoal Face Wash</t>
   </si>
   <si>
-    <t>Broad Spectrum SPF 21 Moisturizer</t>
-  </si>
-  <si>
-    <t>Clinique For Men Super Energizer&amp;trade; Anti-Fatigue Depuffing Eye Gel</t>
-  </si>
-  <si>
-    <t>Moisturizing Lotion</t>
-  </si>
-  <si>
-    <t>Repairwear Laser Focus Wrinkle Correcting Eye Cream</t>
-  </si>
-  <si>
     <t>Oil Control Face Wash</t>
   </si>
   <si>
-    <t>Even Better Clinical Brightening Moisturizer</t>
-  </si>
-  <si>
-    <t>Clinique For Men Maximum Hydrator 72-Hour Auto-Replenishing Hydrator</t>
-  </si>
-  <si>
-    <t>Fresh Pressed Daily Booster with Pure Vitamin C 10%</t>
-  </si>
-  <si>
-    <t>Smart Clinical Repair Wrinkle Correcting Rich Cream</t>
-  </si>
-  <si>
     <t>Clinique Pop Liquid&amp;trade; Matte Lip Colour + Primer Lipstick</t>
   </si>
   <si>
@@ -340,22 +349,19 @@
     <t>Clarifying Lotion 1.0 Twice A Day Exfoliator</t>
   </si>
   <si>
+    <t>Aloe Shave Gel</t>
+  </si>
+  <si>
     <t>Take The Day Off Charcoal Cleansing Balm Makeup Remover</t>
   </si>
   <si>
-    <t>Aloe Shave Gel</t>
-  </si>
-  <si>
-    <t>Sparkle Skin Body Exfoliator</t>
-  </si>
-  <si>
     <t>Clarifying Do-Over Peel</t>
   </si>
   <si>
     <t>Fresh Pressed Renewing Powder Cleanser with Pure Vitamin C</t>
   </si>
   <si>
-    <t>Face Scrub</t>
+    <t>Mini Smart Clinical Repair Wrinkle Correcting Cream</t>
   </si>
   <si>
     <t>Clinique Smart Clinical MD Multi-Dimensional Age Transformer Duo Resculpt + Revolumize</t>
@@ -364,57 +370,51 @@
     <t>Deep Comfort Body Butter</t>
   </si>
   <si>
-    <t>Mini Smart Clinical Repair Wrinkle Correcting Cream</t>
-  </si>
-  <si>
     <t>Post-Shave Soother</t>
   </si>
   <si>
-    <t>Clinique For Men&amp;trade; Anti-Age Eye Cream</t>
-  </si>
-  <si>
     <t>Clinique For Men Oil-Free Moisturizer</t>
   </si>
   <si>
+    <t>Repairwear&amp;trade; Intensive Lip Treatment</t>
+  </si>
+  <si>
     <t>Quickliner&amp;trade; For Lips Intense Lip Liner</t>
   </si>
   <si>
-    <t>Repairwear&amp;trade; Intensive Lip Treatment</t>
+    <t>Even Better Glow&amp;trade; Light Reflecting Makeup Broad Spectrum SPF 15 Foundation</t>
   </si>
   <si>
     <t>Beyond Perfecting Super Concealer Camouflage + 24-Hour Wear</t>
   </si>
   <si>
-    <t>Even Better Glow&amp;trade; Light Reflecting Makeup Broad Spectrum SPF 15 Foundation</t>
+    <t>Acne Solutions Cleansing Foam</t>
+  </si>
+  <si>
+    <t>Pep-Start Daily UV Protector Face Sunscreen SPF 50</t>
+  </si>
+  <si>
+    <t>Mini Acne Solutions&amp;trade; Cleansing Foam</t>
+  </si>
+  <si>
+    <t>Mini High Impact High-Fi Full Volume Mascara</t>
   </si>
   <si>
     <t>Turnaround Accelerated Renewal Serum</t>
   </si>
   <si>
-    <t>Acne Solutions Cleansing Foam</t>
-  </si>
-  <si>
-    <t>Pep-Start Daily UV Protector Face Sunscreen SPF 50</t>
-  </si>
-  <si>
-    <t>Mini Acne Solutions&amp;trade; Cleansing Foam</t>
-  </si>
-  <si>
-    <t>Mini High Impact High-Fi Full Volume Mascara</t>
-  </si>
-  <si>
     <t>Superprimer Face Primer - Universal Face Primer</t>
   </si>
   <si>
     <t>4.395</t>
   </si>
   <si>
+    <t>4.2409</t>
+  </si>
+  <si>
     <t>4.2842</t>
   </si>
   <si>
-    <t>4.2409</t>
-  </si>
-  <si>
     <t>4.5132</t>
   </si>
   <si>
@@ -433,22 +433,25 @@
     <t>4.5036</t>
   </si>
   <si>
+    <t>4.1852</t>
+  </si>
+  <si>
     <t>4.3343</t>
   </si>
   <si>
-    <t>4.1852</t>
+    <t>4.5</t>
+  </si>
+  <si>
+    <t>4.4302</t>
+  </si>
+  <si>
+    <t>4.07</t>
   </si>
   <si>
     <t>4.3684</t>
   </si>
   <si>
-    <t>4.4302</t>
-  </si>
-  <si>
-    <t>4.5</t>
-  </si>
-  <si>
-    <t>4.07</t>
+    <t>4.3712</t>
   </si>
   <si>
     <t>4.3667</t>
@@ -463,7 +466,7 @@
     <t>3.7504</t>
   </si>
   <si>
-    <t>4.3712</t>
+    <t>4.3959</t>
   </si>
   <si>
     <t>4.3104</t>
@@ -472,12 +475,12 @@
     <t>3.8922</t>
   </si>
   <si>
-    <t>4.3959</t>
-  </si>
-  <si>
     <t>3.762</t>
   </si>
   <si>
+    <t>3.7662</t>
+  </si>
+  <si>
     <t>4.3557</t>
   </si>
   <si>
@@ -499,87 +502,96 @@
     <t>3.7283</t>
   </si>
   <si>
-    <t>3.7662</t>
+    <t>4.2566</t>
+  </si>
+  <si>
+    <t>4.6092</t>
   </si>
   <si>
     <t>4.3122</t>
   </si>
   <si>
-    <t>4.6092</t>
+    <t>3.6</t>
   </si>
   <si>
     <t>4.037</t>
   </si>
   <si>
-    <t>4.2566</t>
-  </si>
-  <si>
     <t>4.1957</t>
   </si>
   <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>4.1451</t>
+  </si>
+  <si>
+    <t>4.1785</t>
+  </si>
+  <si>
+    <t>4.4301</t>
+  </si>
+  <si>
     <t>3.9487</t>
   </si>
   <si>
-    <t>2.5</t>
-  </si>
-  <si>
-    <t>4.4301</t>
-  </si>
-  <si>
-    <t>3.6</t>
-  </si>
-  <si>
     <t>4.0588</t>
   </si>
   <si>
-    <t>4.1785</t>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>4.0194</t>
   </si>
   <si>
     <t>4.3532</t>
   </si>
   <si>
-    <t>4.1451</t>
+    <t>4.3222</t>
+  </si>
+  <si>
+    <t>3.8825</t>
+  </si>
+  <si>
+    <t>4.5311</t>
+  </si>
+  <si>
+    <t>4.6667</t>
   </si>
   <si>
     <t>4.2806</t>
   </si>
   <si>
-    <t>0.0</t>
-  </si>
-  <si>
-    <t>3.8825</t>
-  </si>
-  <si>
-    <t>4.6667</t>
-  </si>
-  <si>
-    <t>4.3222</t>
-  </si>
-  <si>
     <t>3.9983</t>
   </si>
   <si>
+    <t>3.7907</t>
+  </si>
+  <si>
+    <t>4.1408</t>
+  </si>
+  <si>
+    <t>3.6217</t>
+  </si>
+  <si>
     <t>4.2396</t>
   </si>
   <si>
-    <t>4.0194</t>
-  </si>
-  <si>
-    <t>3.7907</t>
-  </si>
-  <si>
-    <t>4.5311</t>
-  </si>
-  <si>
-    <t>4.1408</t>
-  </si>
-  <si>
-    <t>3.6217</t>
+    <t>4.1111</t>
+  </si>
+  <si>
+    <t>4.4826</t>
   </si>
   <si>
     <t>4.4752</t>
   </si>
   <si>
+    <t>3.413</t>
+  </si>
+  <si>
+    <t>4.5455</t>
+  </si>
+  <si>
     <t>3.3014</t>
   </si>
   <si>
@@ -589,9 +601,6 @@
     <t>4.1235</t>
   </si>
   <si>
-    <t>4.4826</t>
-  </si>
-  <si>
     <t>4.0275</t>
   </si>
   <si>
@@ -601,21 +610,15 @@
     <t>4.6061</t>
   </si>
   <si>
+    <t>3.0995</t>
+  </si>
+  <si>
+    <t>3.9449</t>
+  </si>
+  <si>
     <t>4.5198</t>
   </si>
   <si>
-    <t>3.0995</t>
-  </si>
-  <si>
-    <t>3.413</t>
-  </si>
-  <si>
-    <t>3.9449</t>
-  </si>
-  <si>
-    <t>4.1111</t>
-  </si>
-  <si>
     <t>4.3593</t>
   </si>
   <si>
@@ -625,75 +628,81 @@
     <t>3.68</t>
   </si>
   <si>
+    <t>4.1696</t>
+  </si>
+  <si>
+    <t>4.5417</t>
+  </si>
+  <si>
+    <t>3.8585</t>
+  </si>
+  <si>
+    <t>4.3333</t>
+  </si>
+  <si>
+    <t>4.3701</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>4.1706</t>
+  </si>
+  <si>
+    <t>4.1164</t>
+  </si>
+  <si>
+    <t>4.5257</t>
+  </si>
+  <si>
+    <t>3.2428</t>
+  </si>
+  <si>
+    <t>4.0909</t>
+  </si>
+  <si>
     <t>4.1585</t>
   </si>
   <si>
-    <t>4.1696</t>
-  </si>
-  <si>
-    <t>4.5417</t>
-  </si>
-  <si>
-    <t>4.5455</t>
-  </si>
-  <si>
-    <t>3.8585</t>
-  </si>
-  <si>
-    <t>3.5</t>
-  </si>
-  <si>
-    <t>4.1706</t>
-  </si>
-  <si>
-    <t>4.1164</t>
-  </si>
-  <si>
-    <t>4.5257</t>
-  </si>
-  <si>
-    <t>4.3701</t>
-  </si>
-  <si>
-    <t>3.2428</t>
-  </si>
-  <si>
-    <t>4.0909</t>
-  </si>
-  <si>
     <t>4.3939</t>
   </si>
   <si>
+    <t>4.3529</t>
+  </si>
+  <si>
+    <t>4.3562</t>
+  </si>
+  <si>
+    <t>3.9</t>
+  </si>
+  <si>
+    <t>4.475</t>
+  </si>
+  <si>
+    <t>4.7353</t>
+  </si>
+  <si>
+    <t>3.8947</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>4.4615</t>
+  </si>
+  <si>
+    <t>3.9438</t>
+  </si>
+  <si>
+    <t>4.3158</t>
+  </si>
+  <si>
     <t>4.7407</t>
   </si>
   <si>
-    <t>4.3529</t>
-  </si>
-  <si>
-    <t>3.9</t>
-  </si>
-  <si>
-    <t>4.475</t>
-  </si>
-  <si>
-    <t>3.8947</t>
-  </si>
-  <si>
     <t>4.1667</t>
   </si>
   <si>
-    <t>3.0</t>
-  </si>
-  <si>
-    <t>4.4615</t>
-  </si>
-  <si>
-    <t>3.9438</t>
-  </si>
-  <si>
-    <t>4.3158</t>
-  </si>
-  <si>
     <t>3.6774</t>
   </si>
   <si>
@@ -706,16 +715,13 @@
     <t>4.725</t>
   </si>
   <si>
-    <t>4.3562</t>
-  </si>
-  <si>
     <t>3.2857</t>
   </si>
   <si>
     <t>4.381</t>
   </si>
   <si>
-    <t>4.7353</t>
+    <t>4.2778</t>
   </si>
   <si>
     <t>2.8462</t>
@@ -724,57 +730,51 @@
     <t>4.698</t>
   </si>
   <si>
-    <t>4.2778</t>
-  </si>
-  <si>
     <t>4.6458</t>
   </si>
   <si>
-    <t>4.3333</t>
-  </si>
-  <si>
     <t>4.2083</t>
   </si>
   <si>
+    <t>4.2754</t>
+  </si>
+  <si>
     <t>4.25</t>
   </si>
   <si>
-    <t>4.2754</t>
+    <t>4.3028</t>
   </si>
   <si>
     <t>4.0438</t>
   </si>
   <si>
-    <t>4.3028</t>
+    <t>4.1693</t>
+  </si>
+  <si>
+    <t>4.2513</t>
+  </si>
+  <si>
+    <t>4.125</t>
+  </si>
+  <si>
+    <t>3.25</t>
   </si>
   <si>
     <t>4.3237</t>
   </si>
   <si>
-    <t>4.1693</t>
-  </si>
-  <si>
-    <t>4.2513</t>
-  </si>
-  <si>
-    <t>4.125</t>
-  </si>
-  <si>
-    <t>3.25</t>
-  </si>
-  <si>
     <t>4.2674</t>
   </si>
   <si>
     <t>4521</t>
   </si>
   <si>
+    <t>1868</t>
+  </si>
+  <si>
     <t>2808</t>
   </si>
   <si>
-    <t>1868</t>
-  </si>
-  <si>
     <t>4511</t>
   </si>
   <si>
@@ -793,22 +793,25 @@
     <t>1104</t>
   </si>
   <si>
+    <t>2635</t>
+  </si>
+  <si>
     <t>1379</t>
   </si>
   <si>
-    <t>2635</t>
+    <t>2</t>
+  </si>
+  <si>
+    <t>4042</t>
+  </si>
+  <si>
+    <t>1656</t>
   </si>
   <si>
     <t>2237</t>
   </si>
   <si>
-    <t>4042</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>1656</t>
+    <t>299</t>
   </si>
   <si>
     <t>1399</t>
@@ -823,7 +826,7 @@
     <t>2608</t>
   </si>
   <si>
-    <t>299</t>
+    <t>1018</t>
   </si>
   <si>
     <t>931</t>
@@ -832,12 +835,12 @@
     <t>677</t>
   </si>
   <si>
-    <t>1018</t>
-  </si>
-  <si>
     <t>811</t>
   </si>
   <si>
+    <t>911</t>
+  </si>
+  <si>
     <t>357</t>
   </si>
   <si>
@@ -859,93 +862,96 @@
     <t>92</t>
   </si>
   <si>
-    <t>911</t>
+    <t>1543</t>
+  </si>
+  <si>
+    <t>1213</t>
   </si>
   <si>
     <t>583</t>
   </si>
   <si>
-    <t>1213</t>
+    <t>115</t>
   </si>
   <si>
     <t>27</t>
   </si>
   <si>
-    <t>1543</t>
-  </si>
-  <si>
     <t>1676</t>
   </si>
   <si>
+    <t>1647</t>
+  </si>
+  <si>
+    <t>1905</t>
+  </si>
+  <si>
+    <t>4041</t>
+  </si>
+  <si>
     <t>429</t>
   </si>
   <si>
-    <t>4041</t>
-  </si>
-  <si>
-    <t>115</t>
-  </si>
-  <si>
     <t>51</t>
   </si>
   <si>
-    <t>1905</t>
+    <t>0</t>
+  </si>
+  <si>
+    <t>720</t>
   </si>
   <si>
     <t>637</t>
   </si>
   <si>
-    <t>1647</t>
+    <t>270</t>
+  </si>
+  <si>
+    <t>732</t>
+  </si>
+  <si>
+    <t>819</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
   <si>
     <t>784</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>732</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>270</t>
-  </si>
-  <si>
     <t>592</t>
   </si>
   <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>497</t>
+  </si>
+  <si>
     <t>2024</t>
   </si>
   <si>
-    <t>720</t>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>819</t>
-  </si>
-  <si>
-    <t>71</t>
-  </si>
-  <si>
-    <t>497</t>
+    <t>117</t>
+  </si>
+  <si>
+    <t>489</t>
   </si>
   <si>
     <t>484</t>
   </si>
   <si>
+    <t>11</t>
+  </si>
+  <si>
     <t>146</t>
   </si>
   <si>
     <t>106</t>
   </si>
   <si>
-    <t>489</t>
-  </si>
-  <si>
     <t>255</t>
   </si>
   <si>
@@ -955,18 +961,15 @@
     <t>33</t>
   </si>
   <si>
+    <t>201</t>
+  </si>
+  <si>
+    <t>254</t>
+  </si>
+  <si>
     <t>202</t>
   </si>
   <si>
-    <t>201</t>
-  </si>
-  <si>
-    <t>254</t>
-  </si>
-  <si>
-    <t>117</t>
-  </si>
-  <si>
     <t>231</t>
   </si>
   <si>
@@ -976,39 +979,36 @@
     <t>100</t>
   </si>
   <si>
+    <t>289</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>763</t>
+  </si>
+  <si>
+    <t>127</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>340</t>
+  </si>
+  <si>
+    <t>481</t>
+  </si>
+  <si>
+    <t>253</t>
+  </si>
+  <si>
+    <t>383</t>
+  </si>
+  <si>
     <t>284</t>
   </si>
   <si>
-    <t>289</t>
-  </si>
-  <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>763</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>340</t>
-  </si>
-  <si>
-    <t>481</t>
-  </si>
-  <si>
-    <t>253</t>
-  </si>
-  <si>
-    <t>127</t>
-  </si>
-  <si>
-    <t>383</t>
-  </si>
-  <si>
     <t>165</t>
   </si>
   <si>
@@ -1021,21 +1021,24 @@
     <t>40</t>
   </si>
   <si>
+    <t>170</t>
+  </si>
+  <si>
     <t>152</t>
   </si>
   <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
     <t>18</t>
   </si>
   <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>160</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
     <t>62</t>
   </si>
   <si>
@@ -1048,48 +1051,45 @@
     <t>42</t>
   </si>
   <si>
-    <t>170</t>
-  </si>
-  <si>
     <t>245</t>
   </si>
   <si>
+    <t>276</t>
+  </si>
+  <si>
     <t>20</t>
   </si>
   <si>
-    <t>276</t>
+    <t>142</t>
   </si>
   <si>
     <t>251</t>
   </si>
   <si>
-    <t>142</t>
+    <t>1057</t>
+  </si>
+  <si>
+    <t>378</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
   <si>
     <t>139</t>
   </si>
   <si>
-    <t>1057</t>
-  </si>
-  <si>
-    <t>378</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
     <t>172</t>
   </si>
   <si>
     <t>https://www.sephora.com/product/almost-lipstick-P122751?skuId=70680</t>
   </si>
   <si>
+    <t>https://www.sephora.com/product/clinique-moisture-surge-trade-100-hour-auto-replenishing-hydrator-P468351?skuId=2421725</t>
+  </si>
+  <si>
     <t>https://www.sephora.com/product/high-impact-mascara-P122912?skuId=711267</t>
   </si>
   <si>
-    <t>https://www.sephora.com/product/clinique-moisture-surge-trade-100-hour-auto-replenishing-hydrator-P468351?skuId=2421725</t>
-  </si>
-  <si>
     <t>https://www.sephora.com/product/take-the-day-off-cleansing-balm-P126301?skuId=886267</t>
   </si>
   <si>
@@ -1108,22 +1108,25 @@
     <t>https://www.sephora.com/product/cheek-pop-P384996?skuId=1674910</t>
   </si>
   <si>
+    <t>https://www.sephora.com/product/even-better-makeup-spf-15-P234967?skuId=2083871</t>
+  </si>
+  <si>
     <t>https://www.sephora.com/product/stay-matte-sheer-pressed-powder-P122748?skuId=51573</t>
   </si>
   <si>
-    <t>https://www.sephora.com/product/even-better-makeup-spf-15-P234967?skuId=2083871</t>
+    <t>https://www.sephora.com/product/all-about-shadow-8-pan-palette-P384505?skuId=2702744</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/dramatically-different-moisturizing-gel-P122900?skuId=789727</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/all-about-eyes-P122774?skuId=126581</t>
   </si>
   <si>
     <t>https://www.sephora.com/product/liquid-facial-soap-P139000?skuId=899070</t>
   </si>
   <si>
-    <t>https://www.sephora.com/product/dramatically-different-moisturizing-gel-P122900?skuId=789727</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/all-about-shadow-8-pan-palette-P384505?skuId=2702744</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/all-about-eyes-P122774?skuId=126581</t>
+    <t>https://www.sephora.com/product/high-impact-high-fi-tm-full-volume-mascara-P507084?skuId=2677672</t>
   </si>
   <si>
     <t>https://www.sephora.com/product/clarifying-lotion-2-P122882?skuId=1295708</t>
@@ -1138,7 +1141,7 @@
     <t>https://www.sephora.com/product/beyond-perfecting-foundation-concealer-P393325?skuId=2166833</t>
   </si>
   <si>
-    <t>https://www.sephora.com/product/high-impact-high-fi-tm-full-volume-mascara-P507084?skuId=2677672</t>
+    <t>https://www.sephora.com/product/acne-solutions-clarifying-lotion-P188307?skuId=1027473</t>
   </si>
   <si>
     <t>https://www.sephora.com/product/clarifying-lotion-3-P122881?skuId=1295716</t>
@@ -1147,27 +1150,27 @@
     <t>https://www.sephora.com/product/take-day-off-micellar-cleansing-towelettes-for-face-eyes-P406924?skuId=1802354</t>
   </si>
   <si>
-    <t>https://www.sephora.com/product/acne-solutions-clarifying-lotion-P188307?skuId=1027473</t>
-  </si>
-  <si>
     <t>https://www.sephora.com/product/moisture-surge-cc-cream-hydrating-colour-corrector-broad-spectrum-spf-30-P378639?skuId=1509512</t>
   </si>
   <si>
+    <t>https://www.sephora.com/product/all-about-eyes-serum-de-puffing-eye-massage-P257537?skuId=1234897</t>
+  </si>
+  <si>
     <t>https://www.sephora.com/product/clinique-moisture-surge-tm-broad-spectrum-spf-28-sheer-hydrator-moisturizer-P505507?skuId=2672970</t>
   </si>
   <si>
+    <t>https://www.sephora.com/product/rinse-off-foaming-cleanser-P122762?skuId=47860</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/clinique-even-better-clinical-radical-dark-spot-corrector-interrupter-P455622?skuId=2313401</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/clinique-even-better-clinical-serum-foundation-broad-spectrum-spf-25-P468639?skuId=2422566</t>
+  </si>
+  <si>
     <t>https://www.sephora.com/product/clinique-take-day-off-cleansing-balm-mini-P453816?skuId=2039477</t>
   </si>
   <si>
-    <t>https://www.sephora.com/product/rinse-off-foaming-cleanser-P122762?skuId=47860</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/clinique-even-better-clinical-radical-dark-spot-corrector-interrupter-P455622?skuId=2313401</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/clinique-even-better-clinical-serum-foundation-broad-spectrum-spf-25-P468639?skuId=2422566</t>
-  </si>
-  <si>
     <t>https://www.sephora.com/product/acne-solutions-clinical-clearing-gel-P385432?skuId=1592831</t>
   </si>
   <si>
@@ -1177,90 +1180,99 @@
     <t>https://www.sephora.com/product/clinique-moisture-surge-sheertint-hydrator-broad-spectrum-spf-25-P457692?skuId=2313708</t>
   </si>
   <si>
-    <t>https://www.sephora.com/product/all-about-eyes-serum-de-puffing-eye-massage-P257537?skuId=1234897</t>
+    <t>https://www.sephora.com/product/quickliner-for-eyes-P122765?skuId=557413</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/exfoliating-scrub-P122718?skuId=579490</t>
   </si>
   <si>
     <t>https://www.sephora.com/product/take-the-day-off-cleansing-oil-P384821?skuId=1583426</t>
   </si>
   <si>
-    <t>https://www.sephora.com/product/exfoliating-scrub-P122718?skuId=579490</t>
+    <t>https://www.sephora.com/product/clinique-moisture-surge-trade-intense-72h-lipid-replenishing-hydrator-P463613?skuId=2368694</t>
   </si>
   <si>
     <t>https://www.sephora.com/product/clinique-high-impact-trade-mascara-mini-P479715?skuId=2554525</t>
   </si>
   <si>
-    <t>https://www.sephora.com/product/quickliner-for-eyes-P122765?skuId=557413</t>
-  </si>
-  <si>
     <t>https://www.sephora.com/product/clinique-smart-clinical-repair-trade-wrinkle-correcting-serum-P473267?skuId=2480705</t>
   </si>
   <si>
+    <t>https://www.sephora.com/product/clinique-moisture-megastars-hydrating-skincare-set-P510763?skuId=2766384</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/all-about-eyes-rich-P174502?skuId=971473</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/smart-clinical-repair-wrinkle-correcting-cream-P500718?skuId=2608404</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/dramatically-different-moisturizing-gel-mini-P425860?skuId=789735</t>
+  </si>
+  <si>
     <t>https://www.sephora.com/product/high-impact-waterproof-mascara-P377219?skuId=1487180</t>
   </si>
   <si>
-    <t>https://www.sephora.com/product/clinique-moisture-megastars-hydrating-skincare-set-P510763?skuId=2766384</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/dramatically-different-moisturizing-gel-mini-P425860?skuId=789735</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/clinique-moisture-surge-trade-intense-72h-lipid-replenishing-hydrator-P463613?skuId=2368694</t>
-  </si>
-  <si>
     <t>https://www.sephora.com/product/take-the-day-off-to-go-P223704?skuId=1123116</t>
   </si>
   <si>
-    <t>https://www.sephora.com/product/smart-clinical-repair-wrinkle-correcting-cream-P500718?skuId=2608404</t>
+    <t>https://www.sephora.com/product/all-about-shadow-single-P381916?skuId=2717015</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/acne-solutions-all-over-clearing-treatment-oil-free-P188306?skuId=1027465</t>
   </si>
   <si>
     <t>https://www.sephora.com/product/blended-face-powder-brush-P122668?skuId=51532</t>
   </si>
   <si>
-    <t>https://www.sephora.com/product/all-about-eyes-rich-P174502?skuId=971473</t>
+    <t>https://www.sephora.com/product/dramatically-different-moisturizing-lotion-mini-P425857?skuId=1682343</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/great-skin-great-deal-set-for-combination-oily-skin-P385631?skuId=1599422</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/dramatically-different-hydrating-jelly-P432241?skuId=2240331</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/7-day-scrub-cream-rinse-off-formula-P122661?skuId=47936</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/mini-moisture-surge-broad-spectrum-spf-28-sheer-hydrator-moisturizer-P508604?skuId=2694875</t>
   </si>
   <si>
     <t>https://www.sephora.com/product/lash-building-primer-P122866?skuId=741967</t>
   </si>
   <si>
-    <t>https://www.sephora.com/product/all-about-shadow-single-P381916?skuId=2717015</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/dramatically-different-moisturizing-lotion-mini-P425857?skuId=1682343</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/dramatically-different-hydrating-jelly-P432241?skuId=2240331</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/mini-moisture-surge-broad-spectrum-spf-28-sheer-hydrator-moisturizer-P508604?skuId=2694875</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/great-skin-great-deal-set-for-combination-oily-skin-P385631?skuId=1599422</t>
-  </si>
-  <si>
     <t>https://www.sephora.com/product/redness-solutions-daily-relief-cream-P201440?skuId=1066729</t>
   </si>
   <si>
+    <t>https://www.sephora.com/product/clinique-high-impact-tm-easy-liquid-liner-P481064?skuId=2515245</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/clinique-mini-moisture-surge-trade-100-hour-auto-replenishing-hydrator-P468818?skuId=2421683</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/high-impact-extreme-volume-mascara-P374580?skuId=1440486</t>
+  </si>
+  <si>
     <t>https://www.sephora.com/product/clinique-smart-clinical-repair-trade-wrinkle-correcting-eye-cream-P479734?skuId=2531697</t>
   </si>
   <si>
-    <t>https://www.sephora.com/product/acne-solutions-all-over-clearing-treatment-oil-free-P188306?skuId=1027465</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/clinique-high-impact-tm-easy-liquid-liner-P481064?skuId=2515245</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/7-day-scrub-cream-rinse-off-formula-P122661?skuId=47936</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/clinique-mini-moisture-surge-trade-100-hour-auto-replenishing-hydrator-P468818?skuId=2421683</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/high-impact-extreme-volume-mascara-P374580?skuId=1440486</t>
+    <t>https://www.sephora.com/product/acne-solutions-acne-line-correcting-serum-P407040?skuId=1802321</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/clinique-take-day-off-tm-facial-cleansing-mousse-P510025?skuId=2734507</t>
   </si>
   <si>
     <t>https://www.sephora.com/product/moisture-surge-overnight-mask-P377577?skuId=1484641</t>
   </si>
   <si>
+    <t>https://www.sephora.com/product/broad-spectrum-spf-50-mineral-sunscreen-fluid-for-face-P410101?skuId=1809383</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/anti-age-moisturizer-P385254?skuId=1596220</t>
+  </si>
+  <si>
     <t>https://www.sephora.com/product/moisture-surge-eye-96-hour-hydro-filler-concentrate-P443383?skuId=2171940</t>
   </si>
   <si>
@@ -1270,9 +1282,6 @@
     <t>https://www.sephora.com/product/blackhead-solutions-7-day-deep-pore-cleanse-scrub-P432242?skuId=2083780</t>
   </si>
   <si>
-    <t>https://www.sephora.com/product/clinique-take-day-off-tm-facial-cleansing-mousse-P510025?skuId=2734507</t>
-  </si>
-  <si>
     <t>https://www.sephora.com/product/moisture-surge-hydrating-supercharged-concentrate-P417984?skuId=1898790</t>
   </si>
   <si>
@@ -1282,24 +1291,18 @@
     <t>https://www.sephora.com/product/clinique-all-about-clean-trade-2-in-1-cleansing-exfoliating-jelly-P469451?skuId=2421766</t>
   </si>
   <si>
+    <t>https://www.sephora.com/product/blackhead-solutions-self-heating-blackhead-extractor-P432243?skuId=2083798</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/acne-solutions-clinical-clearing-gel-mini-P425858?skuId=1592856</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/broad-spectrum-spf-50-sunscreen-face-cream-P232327?skuId=1151711</t>
+  </si>
+  <si>
     <t>https://www.sephora.com/product/clarifying-lotion-1-P122651?skuId=1295690</t>
   </si>
   <si>
-    <t>https://www.sephora.com/product/blackhead-solutions-self-heating-blackhead-extractor-P432243?skuId=2083798</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/acne-solutions-clinical-clearing-gel-mini-P425858?skuId=1592856</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/broad-spectrum-spf-50-mineral-sunscreen-fluid-for-face-P410101?skuId=1809383</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/broad-spectrum-spf-50-sunscreen-face-cream-P232327?skuId=1151711</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/acne-solutions-acne-line-correcting-serum-P407040?skuId=1802321</t>
-  </si>
-  <si>
     <t>https://www.sephora.com/product/clarifying-lotion-4-P122876?skuId=1295724</t>
   </si>
   <si>
@@ -1309,75 +1312,81 @@
     <t>https://www.sephora.com/product/clinique-superdefense-city-block-spf-50-daily-energy-face-protector-P456991?skuId=2313757</t>
   </si>
   <si>
+    <t>https://www.sephora.com/product/redness-solutions-soothing-cleanser-P201439?skuId=1066711</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/exfoliating-tonic-P122761?skuId=50765</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/age-defense-bb-cream-broad-spectrum-spf-30-P293010?skuId=1417302</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/anti-age-eye-cream-P257804?skuId=1202464</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/marimekko-clinique-pop-splash-lip-gloss-P428662?skuId=2023471</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/clinique-even-better-brightening-moisturizer-spf-20-P504674?skuId=2664365</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/clinique-mini-take-day-off-charcoal-cleansing-balm-makeup-remover-P503737?skuId=2641876</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/city-block-sheer-oil-free-daily-face-protector-spf-25-P196542?skuId=999565</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/true-bronze-pressed-powder-bronzer-P122807?skuId=847517</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/even-better-eyes-dark-circle-corrector-P374841?skuId=1438787</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/clinique-all-about-clean-trade-2-in-1-charcoal-mask-scrub-P469452?skuId=2421774</t>
+  </si>
+  <si>
     <t>https://www.sephora.com/product/repairwear-anti-gravity-eye-lift-cream-P122727?skuId=502443</t>
   </si>
   <si>
-    <t>https://www.sephora.com/product/redness-solutions-soothing-cleanser-P201439?skuId=1066711</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/exfoliating-tonic-P122761?skuId=50765</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/anti-age-moisturizer-P385254?skuId=1596220</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/age-defense-bb-cream-broad-spectrum-spf-30-P293010?skuId=1417302</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/clinique-even-better-brightening-moisturizer-spf-20-P504674?skuId=2664365</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/clinique-mini-take-day-off-charcoal-cleansing-balm-makeup-remover-P503737?skuId=2641876</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/city-block-sheer-oil-free-daily-face-protector-spf-25-P196542?skuId=999565</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/true-bronze-pressed-powder-bronzer-P122807?skuId=847517</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/marimekko-clinique-pop-splash-lip-gloss-P428662?skuId=2023471</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/even-better-eyes-dark-circle-corrector-P374841?skuId=1438787</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/clinique-all-about-clean-trade-2-in-1-charcoal-mask-scrub-P469452?skuId=2421774</t>
-  </si>
-  <si>
     <t>https://www.sephora.com/product/dramatically-different-moisturizing-cream-P398717?skuId=1717016</t>
   </si>
   <si>
+    <t>https://www.sephora.com/product/broad-spectrum-spf-21-moisturizer-P122806?skuId=882506</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/sparkle-skin-body-exfoliator-P122749?skuId=410712</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/clinique-for-men-super-energizer-anti-fatigue-depuffing-eye-gel-P435207?skuId=2111904</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/moisturizing-lotion-P122809?skuId=1580794</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/face-scrub-P122665?skuId=50997</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/repairwear-laser-focus-wrinkle-correcting-eye-cream-P377576?skuId=1484625</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/clinique-even-better-clinical-brightening-moisturizer-P506372?skuId=2672988</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/clinique-for-men-maximum-hydrator-72-hour-auto-replenishing-hydrator-P448561?skuId=2240349</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/fresh-pressed-daily-booster-with-pure-vitamin-c-10-P416824?skuId=1898774</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/smart-clinical-repair-wrinkle-correcting-rich-cream-P500771?skuId=2608396</t>
+  </si>
+  <si>
     <t>https://www.sephora.com/product/charcoal-face-wash-P398713?skuId=1734649</t>
   </si>
   <si>
-    <t>https://www.sephora.com/product/broad-spectrum-spf-21-moisturizer-P122806?skuId=882506</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/clinique-for-men-super-energizer-anti-fatigue-depuffing-eye-gel-P435207?skuId=2111904</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/moisturizing-lotion-P122809?skuId=1580794</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/repairwear-laser-focus-wrinkle-correcting-eye-cream-P377576?skuId=1484625</t>
-  </si>
-  <si>
     <t>https://www.sephora.com/product/oil-control-face-wash-P385256?skuId=1580778</t>
   </si>
   <si>
-    <t>https://www.sephora.com/product/clinique-even-better-clinical-brightening-moisturizer-P506372?skuId=2672988</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/clinique-for-men-maximum-hydrator-72-hour-auto-replenishing-hydrator-P448561?skuId=2240349</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/fresh-pressed-daily-booster-with-pure-vitamin-c-10-P416824?skuId=1898774</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/smart-clinical-repair-wrinkle-correcting-rich-cream-P500771?skuId=2608396</t>
-  </si>
-  <si>
     <t>https://www.sephora.com/product/pop-liquid-matte-lip-colour-P411531?skuId=1860220</t>
   </si>
   <si>
@@ -1387,22 +1396,19 @@
     <t>https://www.sephora.com/product/clarifying-lotion-1-0-twice-day-exfoliator-P409920?skuId=1829514</t>
   </si>
   <si>
+    <t>https://www.sephora.com/product/aloe-shave-gel-P122682?skuId=1580810</t>
+  </si>
+  <si>
     <t>https://www.sephora.com/product/clinique-take-day-off-charcoal-cleansing-balm-makeup-remover-P503747?skuId=2641884</t>
   </si>
   <si>
-    <t>https://www.sephora.com/product/aloe-shave-gel-P122682?skuId=1580810</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/sparkle-skin-body-exfoliator-P122749?skuId=410712</t>
-  </si>
-  <si>
     <t>https://www.sephora.com/product/clinique-clarifying-do-over-peel-P481668?skuId=2531739</t>
   </si>
   <si>
     <t>https://www.sephora.com/product/fresh-pressed-renewing-powder-cleanser-P417323?skuId=1898782</t>
   </si>
   <si>
-    <t>https://www.sephora.com/product/face-scrub-P122665?skuId=50997</t>
+    <t>https://www.sephora.com/product/mini-smart-clinical-repair-wrinkle-correcting-cream-P500790?skuId=2608503</t>
   </si>
   <si>
     <t>https://www.sephora.com/product/clinique-smart-clinical-md-multi-dimensional-age-transformer-duo-resculpt-revolumize-P448565?skuId=2240323</t>
@@ -1411,57 +1417,51 @@
     <t>https://www.sephora.com/product/deep-comfort-body-butter-P122654?skuId=637025</t>
   </si>
   <si>
-    <t>https://www.sephora.com/product/mini-smart-clinical-repair-wrinkle-correcting-cream-P500790?skuId=2608503</t>
-  </si>
-  <si>
     <t>https://www.sephora.com/product/post-shave-soother-P122770?skuId=51052</t>
   </si>
   <si>
-    <t>https://www.sephora.com/product/anti-age-eye-cream-P257804?skuId=1202464</t>
-  </si>
-  <si>
     <t>https://www.sephora.com/product/oil-control-mattifying-moisturizer-P122683?skuId=1580802</t>
   </si>
   <si>
+    <t>https://www.sephora.com/product/repairwear-intensive-lip-treatment-P122782?skuId=883306</t>
+  </si>
+  <si>
     <t>https://www.sephora.com/product/quickliner-for-lips-intense-P400708?skuId=1719079</t>
   </si>
   <si>
-    <t>https://www.sephora.com/product/repairwear-intensive-lip-treatment-P122782?skuId=883306</t>
+    <t>https://www.sephora.com/product/even-better-trade-glow-light-reflecting-makeup-broad-spectrum-spf-15-P422881?skuId=1953587</t>
   </si>
   <si>
     <t>https://www.sephora.com/product/beyond-perfecting-super-concealer-P421227?skuId=1948207</t>
   </si>
   <si>
-    <t>https://www.sephora.com/product/even-better-trade-glow-light-reflecting-makeup-broad-spectrum-spf-15-P422881?skuId=1953587</t>
+    <t>https://www.sephora.com/product/acne-solutions-cleansing-foam-P188309?skuId=1027507</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/pep-start-daily-uv-protector-broad-spectrum-spf-50-P415773?skuId=1898725</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/clinique-mini-acne-solutions-trade-cleansing-foam-P480289?skuId=2531747</t>
+  </si>
+  <si>
+    <t>https://www.sephora.com/product/clinique-mini-high-impact-high-fi-full-volume-mascara-P510414?skuId=2742872</t>
   </si>
   <si>
     <t>https://www.sephora.com/product/turnaround-revitalizing-serum-P302900?skuId=1689157</t>
   </si>
   <si>
-    <t>https://www.sephora.com/product/acne-solutions-cleansing-foam-P188309?skuId=1027507</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/pep-start-daily-uv-protector-broad-spectrum-spf-50-P415773?skuId=1898725</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/clinique-mini-acne-solutions-trade-cleansing-foam-P480289?skuId=2531747</t>
-  </si>
-  <si>
-    <t>https://www.sephora.com/product/clinique-mini-high-impact-high-fi-full-volume-mascara-P510414?skuId=2742872</t>
-  </si>
-  <si>
     <t>https://www.sephora.com/product/superprimer-face-primer-universal-face-primer-P382504?skuId=1540202</t>
   </si>
   <si>
     <t>70680</t>
   </si>
   <si>
+    <t>2421725</t>
+  </si>
+  <si>
     <t>711267</t>
   </si>
   <si>
-    <t>2421725</t>
-  </si>
-  <si>
     <t>886267</t>
   </si>
   <si>
@@ -1480,22 +1480,25 @@
     <t>1674910</t>
   </si>
   <si>
+    <t>2083871</t>
+  </si>
+  <si>
     <t>51573</t>
   </si>
   <si>
-    <t>2083871</t>
+    <t>2702744</t>
+  </si>
+  <si>
+    <t>789727</t>
+  </si>
+  <si>
+    <t>126581</t>
   </si>
   <si>
     <t>899070</t>
   </si>
   <si>
-    <t>789727</t>
-  </si>
-  <si>
-    <t>2702744</t>
-  </si>
-  <si>
-    <t>126581</t>
+    <t>2677672</t>
   </si>
   <si>
     <t>1295708</t>
@@ -1510,7 +1513,7 @@
     <t>2166833</t>
   </si>
   <si>
-    <t>2677672</t>
+    <t>1027473</t>
   </si>
   <si>
     <t>1295716</t>
@@ -1519,27 +1522,27 @@
     <t>1802354</t>
   </si>
   <si>
-    <t>1027473</t>
-  </si>
-  <si>
     <t>1509512</t>
   </si>
   <si>
+    <t>1234897</t>
+  </si>
+  <si>
     <t>2672970</t>
   </si>
   <si>
+    <t>47860</t>
+  </si>
+  <si>
+    <t>2313401</t>
+  </si>
+  <si>
+    <t>2422566</t>
+  </si>
+  <si>
     <t>2039477</t>
   </si>
   <si>
-    <t>47860</t>
-  </si>
-  <si>
-    <t>2313401</t>
-  </si>
-  <si>
-    <t>2422566</t>
-  </si>
-  <si>
     <t>1592831</t>
   </si>
   <si>
@@ -1549,90 +1552,99 @@
     <t>2313708</t>
   </si>
   <si>
-    <t>1234897</t>
+    <t>557413</t>
+  </si>
+  <si>
+    <t>579490</t>
   </si>
   <si>
     <t>1583426</t>
   </si>
   <si>
-    <t>579490</t>
+    <t>2368694</t>
   </si>
   <si>
     <t>2554525</t>
   </si>
   <si>
-    <t>557413</t>
-  </si>
-  <si>
     <t>2480705</t>
   </si>
   <si>
+    <t>2766384</t>
+  </si>
+  <si>
+    <t>971473</t>
+  </si>
+  <si>
+    <t>2608404</t>
+  </si>
+  <si>
+    <t>789735</t>
+  </si>
+  <si>
     <t>1487180</t>
   </si>
   <si>
-    <t>2766384</t>
-  </si>
-  <si>
-    <t>789735</t>
-  </si>
-  <si>
-    <t>2368694</t>
-  </si>
-  <si>
     <t>1123116</t>
   </si>
   <si>
-    <t>2608404</t>
+    <t>2717015</t>
+  </si>
+  <si>
+    <t>1027465</t>
   </si>
   <si>
     <t>51532</t>
   </si>
   <si>
-    <t>971473</t>
+    <t>1682343</t>
+  </si>
+  <si>
+    <t>1599422</t>
+  </si>
+  <si>
+    <t>2240331</t>
+  </si>
+  <si>
+    <t>47936</t>
+  </si>
+  <si>
+    <t>2694875</t>
   </si>
   <si>
     <t>741967</t>
   </si>
   <si>
-    <t>2717015</t>
-  </si>
-  <si>
-    <t>1682343</t>
-  </si>
-  <si>
-    <t>2240331</t>
-  </si>
-  <si>
-    <t>2694875</t>
-  </si>
-  <si>
-    <t>1599422</t>
-  </si>
-  <si>
     <t>1066729</t>
   </si>
   <si>
+    <t>2515245</t>
+  </si>
+  <si>
+    <t>2421683</t>
+  </si>
+  <si>
+    <t>1440486</t>
+  </si>
+  <si>
     <t>2531697</t>
   </si>
   <si>
-    <t>1027465</t>
-  </si>
-  <si>
-    <t>2515245</t>
-  </si>
-  <si>
-    <t>47936</t>
-  </si>
-  <si>
-    <t>2421683</t>
-  </si>
-  <si>
-    <t>1440486</t>
+    <t>1802321</t>
+  </si>
+  <si>
+    <t>2734507</t>
   </si>
   <si>
     <t>1484641</t>
   </si>
   <si>
+    <t>1809383</t>
+  </si>
+  <si>
+    <t>1596220</t>
+  </si>
+  <si>
     <t>2171940</t>
   </si>
   <si>
@@ -1642,9 +1654,6 @@
     <t>2083780</t>
   </si>
   <si>
-    <t>2734507</t>
-  </si>
-  <si>
     <t>1898790</t>
   </si>
   <si>
@@ -1654,24 +1663,18 @@
     <t>2421766</t>
   </si>
   <si>
+    <t>2083798</t>
+  </si>
+  <si>
+    <t>1592856</t>
+  </si>
+  <si>
+    <t>1151711</t>
+  </si>
+  <si>
     <t>1295690</t>
   </si>
   <si>
-    <t>2083798</t>
-  </si>
-  <si>
-    <t>1592856</t>
-  </si>
-  <si>
-    <t>1809383</t>
-  </si>
-  <si>
-    <t>1151711</t>
-  </si>
-  <si>
-    <t>1802321</t>
-  </si>
-  <si>
     <t>1295724</t>
   </si>
   <si>
@@ -1681,75 +1684,81 @@
     <t>2313757</t>
   </si>
   <si>
+    <t>1066711</t>
+  </si>
+  <si>
+    <t>50765</t>
+  </si>
+  <si>
+    <t>1417302</t>
+  </si>
+  <si>
+    <t>1202464</t>
+  </si>
+  <si>
+    <t>2023471</t>
+  </si>
+  <si>
+    <t>2664365</t>
+  </si>
+  <si>
+    <t>2641876</t>
+  </si>
+  <si>
+    <t>999565</t>
+  </si>
+  <si>
+    <t>847517</t>
+  </si>
+  <si>
+    <t>1438787</t>
+  </si>
+  <si>
+    <t>2421774</t>
+  </si>
+  <si>
     <t>502443</t>
   </si>
   <si>
-    <t>1066711</t>
-  </si>
-  <si>
-    <t>50765</t>
-  </si>
-  <si>
-    <t>1596220</t>
-  </si>
-  <si>
-    <t>1417302</t>
-  </si>
-  <si>
-    <t>2664365</t>
-  </si>
-  <si>
-    <t>2641876</t>
-  </si>
-  <si>
-    <t>999565</t>
-  </si>
-  <si>
-    <t>847517</t>
-  </si>
-  <si>
-    <t>2023471</t>
-  </si>
-  <si>
-    <t>1438787</t>
-  </si>
-  <si>
-    <t>2421774</t>
-  </si>
-  <si>
     <t>1717016</t>
   </si>
   <si>
+    <t>882506</t>
+  </si>
+  <si>
+    <t>410712</t>
+  </si>
+  <si>
+    <t>2111904</t>
+  </si>
+  <si>
+    <t>1580794</t>
+  </si>
+  <si>
+    <t>50997</t>
+  </si>
+  <si>
+    <t>1484625</t>
+  </si>
+  <si>
+    <t>2672988</t>
+  </si>
+  <si>
+    <t>2240349</t>
+  </si>
+  <si>
+    <t>1898774</t>
+  </si>
+  <si>
+    <t>2608396</t>
+  </si>
+  <si>
     <t>1734649</t>
   </si>
   <si>
-    <t>882506</t>
-  </si>
-  <si>
-    <t>2111904</t>
-  </si>
-  <si>
-    <t>1580794</t>
-  </si>
-  <si>
-    <t>1484625</t>
-  </si>
-  <si>
     <t>1580778</t>
   </si>
   <si>
-    <t>2672988</t>
-  </si>
-  <si>
-    <t>2240349</t>
-  </si>
-  <si>
-    <t>1898774</t>
-  </si>
-  <si>
-    <t>2608396</t>
-  </si>
-  <si>
     <t>1860220</t>
   </si>
   <si>
@@ -1759,22 +1768,19 @@
     <t>1829514</t>
   </si>
   <si>
+    <t>1580810</t>
+  </si>
+  <si>
     <t>2641884</t>
   </si>
   <si>
-    <t>1580810</t>
-  </si>
-  <si>
-    <t>410712</t>
-  </si>
-  <si>
     <t>2531739</t>
   </si>
   <si>
     <t>1898782</t>
   </si>
   <si>
-    <t>50997</t>
+    <t>2608503</t>
   </si>
   <si>
     <t>2240323</t>
@@ -1783,57 +1789,51 @@
     <t>637025</t>
   </si>
   <si>
-    <t>2608503</t>
-  </si>
-  <si>
     <t>51052</t>
   </si>
   <si>
-    <t>1202464</t>
-  </si>
-  <si>
     <t>1580802</t>
   </si>
   <si>
+    <t>883306</t>
+  </si>
+  <si>
     <t>1719079</t>
   </si>
   <si>
-    <t>883306</t>
+    <t>1953587</t>
   </si>
   <si>
     <t>1948207</t>
   </si>
   <si>
-    <t>1953587</t>
+    <t>1027507</t>
+  </si>
+  <si>
+    <t>1898725</t>
+  </si>
+  <si>
+    <t>2531747</t>
+  </si>
+  <si>
+    <t>2742872</t>
   </si>
   <si>
     <t>1689157</t>
   </si>
   <si>
-    <t>1027507</t>
-  </si>
-  <si>
-    <t>1898725</t>
-  </si>
-  <si>
-    <t>2531747</t>
-  </si>
-  <si>
-    <t>2742872</t>
-  </si>
-  <si>
     <t>1540202</t>
   </si>
   <si>
     <t>P122751</t>
   </si>
   <si>
+    <t>P468351</t>
+  </si>
+  <si>
     <t>P122912</t>
   </si>
   <si>
-    <t>P468351</t>
-  </si>
-  <si>
     <t>P126301</t>
   </si>
   <si>
@@ -1852,22 +1852,25 @@
     <t>P384996</t>
   </si>
   <si>
+    <t>P234967</t>
+  </si>
+  <si>
     <t>P122748</t>
   </si>
   <si>
-    <t>P234967</t>
+    <t>P384505</t>
+  </si>
+  <si>
+    <t>P122900</t>
+  </si>
+  <si>
+    <t>P122774</t>
   </si>
   <si>
     <t>P139000</t>
   </si>
   <si>
-    <t>P122900</t>
-  </si>
-  <si>
-    <t>P384505</t>
-  </si>
-  <si>
-    <t>P122774</t>
+    <t>P507084</t>
   </si>
   <si>
     <t>P122882</t>
@@ -1882,7 +1885,7 @@
     <t>P393325</t>
   </si>
   <si>
-    <t>P507084</t>
+    <t>P188307</t>
   </si>
   <si>
     <t>P122881</t>
@@ -1891,27 +1894,27 @@
     <t>P406924</t>
   </si>
   <si>
-    <t>P188307</t>
-  </si>
-  <si>
     <t>P378639</t>
   </si>
   <si>
+    <t>P257537</t>
+  </si>
+  <si>
     <t>P505507</t>
   </si>
   <si>
+    <t>P122762</t>
+  </si>
+  <si>
+    <t>P455622</t>
+  </si>
+  <si>
+    <t>P468639</t>
+  </si>
+  <si>
     <t>P453816</t>
   </si>
   <si>
-    <t>P122762</t>
-  </si>
-  <si>
-    <t>P455622</t>
-  </si>
-  <si>
-    <t>P468639</t>
-  </si>
-  <si>
     <t>P385432</t>
   </si>
   <si>
@@ -1921,90 +1924,99 @@
     <t>P457692</t>
   </si>
   <si>
-    <t>P257537</t>
+    <t>P122765</t>
+  </si>
+  <si>
+    <t>P122718</t>
   </si>
   <si>
     <t>P384821</t>
   </si>
   <si>
-    <t>P122718</t>
+    <t>P463613</t>
   </si>
   <si>
     <t>P479715</t>
   </si>
   <si>
-    <t>P122765</t>
-  </si>
-  <si>
     <t>P473267</t>
   </si>
   <si>
+    <t>P510763</t>
+  </si>
+  <si>
+    <t>P174502</t>
+  </si>
+  <si>
+    <t>P500718</t>
+  </si>
+  <si>
+    <t>P425860</t>
+  </si>
+  <si>
     <t>P377219</t>
   </si>
   <si>
-    <t>P510763</t>
-  </si>
-  <si>
-    <t>P425860</t>
-  </si>
-  <si>
-    <t>P463613</t>
-  </si>
-  <si>
     <t>P223704</t>
   </si>
   <si>
-    <t>P500718</t>
+    <t>P381916</t>
+  </si>
+  <si>
+    <t>P188306</t>
   </si>
   <si>
     <t>P122668</t>
   </si>
   <si>
-    <t>P174502</t>
+    <t>P425857</t>
+  </si>
+  <si>
+    <t>P385631</t>
+  </si>
+  <si>
+    <t>P432241</t>
+  </si>
+  <si>
+    <t>P122661</t>
+  </si>
+  <si>
+    <t>P508604</t>
   </si>
   <si>
     <t>P122866</t>
   </si>
   <si>
-    <t>P381916</t>
-  </si>
-  <si>
-    <t>P425857</t>
-  </si>
-  <si>
-    <t>P432241</t>
-  </si>
-  <si>
-    <t>P508604</t>
-  </si>
-  <si>
-    <t>P385631</t>
-  </si>
-  <si>
     <t>P201440</t>
   </si>
   <si>
+    <t>P481064</t>
+  </si>
+  <si>
+    <t>P468818</t>
+  </si>
+  <si>
+    <t>P374580</t>
+  </si>
+  <si>
     <t>P479734</t>
   </si>
   <si>
-    <t>P188306</t>
-  </si>
-  <si>
-    <t>P481064</t>
-  </si>
-  <si>
-    <t>P122661</t>
-  </si>
-  <si>
-    <t>P468818</t>
-  </si>
-  <si>
-    <t>P374580</t>
+    <t>P407040</t>
+  </si>
+  <si>
+    <t>P510025</t>
   </si>
   <si>
     <t>P377577</t>
   </si>
   <si>
+    <t>P410101</t>
+  </si>
+  <si>
+    <t>P385254</t>
+  </si>
+  <si>
     <t>P443383</t>
   </si>
   <si>
@@ -2014,9 +2026,6 @@
     <t>P432242</t>
   </si>
   <si>
-    <t>P510025</t>
-  </si>
-  <si>
     <t>P417984</t>
   </si>
   <si>
@@ -2026,24 +2035,18 @@
     <t>P469451</t>
   </si>
   <si>
+    <t>P432243</t>
+  </si>
+  <si>
+    <t>P425858</t>
+  </si>
+  <si>
+    <t>P232327</t>
+  </si>
+  <si>
     <t>P122651</t>
   </si>
   <si>
-    <t>P432243</t>
-  </si>
-  <si>
-    <t>P425858</t>
-  </si>
-  <si>
-    <t>P410101</t>
-  </si>
-  <si>
-    <t>P232327</t>
-  </si>
-  <si>
-    <t>P407040</t>
-  </si>
-  <si>
     <t>P122876</t>
   </si>
   <si>
@@ -2053,75 +2056,81 @@
     <t>P456991</t>
   </si>
   <si>
+    <t>P201439</t>
+  </si>
+  <si>
+    <t>P122761</t>
+  </si>
+  <si>
+    <t>P293010</t>
+  </si>
+  <si>
+    <t>P257804</t>
+  </si>
+  <si>
+    <t>P428662</t>
+  </si>
+  <si>
+    <t>P504674</t>
+  </si>
+  <si>
+    <t>P503737</t>
+  </si>
+  <si>
+    <t>P196542</t>
+  </si>
+  <si>
+    <t>P122807</t>
+  </si>
+  <si>
+    <t>P374841</t>
+  </si>
+  <si>
+    <t>P469452</t>
+  </si>
+  <si>
     <t>P122727</t>
   </si>
   <si>
-    <t>P201439</t>
-  </si>
-  <si>
-    <t>P122761</t>
-  </si>
-  <si>
-    <t>P385254</t>
-  </si>
-  <si>
-    <t>P293010</t>
-  </si>
-  <si>
-    <t>P504674</t>
-  </si>
-  <si>
-    <t>P503737</t>
-  </si>
-  <si>
-    <t>P196542</t>
-  </si>
-  <si>
-    <t>P122807</t>
-  </si>
-  <si>
-    <t>P428662</t>
-  </si>
-  <si>
-    <t>P374841</t>
-  </si>
-  <si>
-    <t>P469452</t>
-  </si>
-  <si>
     <t>P398717</t>
   </si>
   <si>
+    <t>P122806</t>
+  </si>
+  <si>
+    <t>P122749</t>
+  </si>
+  <si>
+    <t>P435207</t>
+  </si>
+  <si>
+    <t>P122809</t>
+  </si>
+  <si>
+    <t>P122665</t>
+  </si>
+  <si>
+    <t>P377576</t>
+  </si>
+  <si>
+    <t>P506372</t>
+  </si>
+  <si>
+    <t>P448561</t>
+  </si>
+  <si>
+    <t>P416824</t>
+  </si>
+  <si>
+    <t>P500771</t>
+  </si>
+  <si>
     <t>P398713</t>
   </si>
   <si>
-    <t>P122806</t>
-  </si>
-  <si>
-    <t>P435207</t>
-  </si>
-  <si>
-    <t>P122809</t>
-  </si>
-  <si>
-    <t>P377576</t>
-  </si>
-  <si>
     <t>P385256</t>
   </si>
   <si>
-    <t>P506372</t>
-  </si>
-  <si>
-    <t>P448561</t>
-  </si>
-  <si>
-    <t>P416824</t>
-  </si>
-  <si>
-    <t>P500771</t>
-  </si>
-  <si>
     <t>P411531</t>
   </si>
   <si>
@@ -2131,22 +2140,19 @@
     <t>P409920</t>
   </si>
   <si>
+    <t>P122682</t>
+  </si>
+  <si>
     <t>P503747</t>
   </si>
   <si>
-    <t>P122682</t>
-  </si>
-  <si>
-    <t>P122749</t>
-  </si>
-  <si>
     <t>P481668</t>
   </si>
   <si>
     <t>P417323</t>
   </si>
   <si>
-    <t>P122665</t>
+    <t>P500790</t>
   </si>
   <si>
     <t>P448565</t>
@@ -2155,43 +2161,37 @@
     <t>P122654</t>
   </si>
   <si>
-    <t>P500790</t>
-  </si>
-  <si>
     <t>P122770</t>
   </si>
   <si>
-    <t>P257804</t>
-  </si>
-  <si>
     <t>P122683</t>
   </si>
   <si>
+    <t>P122782</t>
+  </si>
+  <si>
     <t>P400708</t>
   </si>
   <si>
-    <t>P122782</t>
+    <t>P422881</t>
   </si>
   <si>
     <t>P421227</t>
   </si>
   <si>
-    <t>P422881</t>
+    <t>P188309</t>
+  </si>
+  <si>
+    <t>P415773</t>
+  </si>
+  <si>
+    <t>P480289</t>
+  </si>
+  <si>
+    <t>P510414</t>
   </si>
   <si>
     <t>P302900</t>
-  </si>
-  <si>
-    <t>P188309</t>
-  </si>
-  <si>
-    <t>P415773</t>
-  </si>
-  <si>
-    <t>P480289</t>
-  </si>
-  <si>
-    <t>P510414</t>
   </si>
   <si>
     <t>P382504</t>
@@ -3096,10 +3096,10 @@
         <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
       <c r="C27" t="s">
-        <v>253</v>
+        <v>275</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>380</v>
@@ -3116,10 +3116,10 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C28" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>381</v>
@@ -3136,10 +3136,10 @@
         <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C29" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>382</v>
@@ -3156,10 +3156,10 @@
         <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C30" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>383</v>
@@ -3176,10 +3176,10 @@
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="C31" t="s">
-        <v>278</v>
+        <v>253</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>384</v>
@@ -3379,7 +3379,7 @@
         <v>168</v>
       </c>
       <c r="C41" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>394</v>
@@ -3839,7 +3839,7 @@
         <v>190</v>
       </c>
       <c r="C64" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>417</v>
@@ -3919,7 +3919,7 @@
         <v>194</v>
       </c>
       <c r="C68" t="s">
-        <v>312</v>
+        <v>284</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>421</v>
@@ -3939,7 +3939,7 @@
         <v>195</v>
       </c>
       <c r="C69" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>422</v>
@@ -3959,7 +3959,7 @@
         <v>196</v>
       </c>
       <c r="C70" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>423</v>
@@ -3976,10 +3976,10 @@
         <v>75</v>
       </c>
       <c r="B71" t="s">
-        <v>158</v>
+        <v>197</v>
       </c>
       <c r="C71" t="s">
-        <v>278</v>
+        <v>314</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>424</v>
@@ -3996,10 +3996,10 @@
         <v>76</v>
       </c>
       <c r="B72" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C72" t="s">
-        <v>280</v>
+        <v>315</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>425</v>
@@ -4016,10 +4016,10 @@
         <v>77</v>
       </c>
       <c r="B73" t="s">
-        <v>198</v>
+        <v>159</v>
       </c>
       <c r="C73" t="s">
-        <v>315</v>
+        <v>279</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>426</v>
@@ -4199,7 +4199,7 @@
         <v>207</v>
       </c>
       <c r="C82" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>435</v>
@@ -4219,7 +4219,7 @@
         <v>208</v>
       </c>
       <c r="C83" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>436</v>
@@ -4239,7 +4239,7 @@
         <v>209</v>
       </c>
       <c r="C84" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>437</v>
@@ -4259,7 +4259,7 @@
         <v>210</v>
       </c>
       <c r="C85" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>438</v>
@@ -4279,7 +4279,7 @@
         <v>211</v>
       </c>
       <c r="C86" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>439</v>
@@ -4299,7 +4299,7 @@
         <v>212</v>
       </c>
       <c r="C87" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>440</v>
@@ -4319,7 +4319,7 @@
         <v>213</v>
       </c>
       <c r="C88" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>441</v>
@@ -4339,7 +4339,7 @@
         <v>214</v>
       </c>
       <c r="C89" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>442</v>
@@ -4359,7 +4359,7 @@
         <v>215</v>
       </c>
       <c r="C90" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>443</v>
@@ -4379,7 +4379,7 @@
         <v>216</v>
       </c>
       <c r="C91" t="s">
-        <v>284</v>
+        <v>331</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>444</v>
@@ -4419,7 +4419,7 @@
         <v>218</v>
       </c>
       <c r="C93" t="s">
-        <v>333</v>
+        <v>310</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>446</v>
@@ -4439,7 +4439,7 @@
         <v>219</v>
       </c>
       <c r="C94" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>447</v>
@@ -4459,7 +4459,7 @@
         <v>220</v>
       </c>
       <c r="C95" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>448</v>
@@ -4479,7 +4479,7 @@
         <v>221</v>
       </c>
       <c r="C96" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>449</v>
@@ -4499,7 +4499,7 @@
         <v>222</v>
       </c>
       <c r="C97" t="s">
-        <v>263</v>
+        <v>336</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>450</v>
@@ -4519,7 +4519,7 @@
         <v>223</v>
       </c>
       <c r="C98" t="s">
-        <v>337</v>
+        <v>261</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>451</v>
@@ -4539,7 +4539,7 @@
         <v>224</v>
       </c>
       <c r="C99" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>452</v>
@@ -4559,7 +4559,7 @@
         <v>225</v>
       </c>
       <c r="C100" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>453</v>
@@ -4579,7 +4579,7 @@
         <v>226</v>
       </c>
       <c r="C101" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>454</v>
@@ -4599,7 +4599,7 @@
         <v>227</v>
       </c>
       <c r="C102" t="s">
-        <v>341</v>
+        <v>286</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>455</v>
@@ -4619,7 +4619,7 @@
         <v>228</v>
       </c>
       <c r="C103" t="s">
-        <v>302</v>
+        <v>340</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>456</v>
@@ -4636,10 +4636,10 @@
         <v>108</v>
       </c>
       <c r="B104" t="s">
-        <v>209</v>
+        <v>229</v>
       </c>
       <c r="C104" t="s">
-        <v>326</v>
+        <v>341</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>457</v>
@@ -4656,10 +4656,10 @@
         <v>109</v>
       </c>
       <c r="B105" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C105" t="s">
-        <v>334</v>
+        <v>342</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>458</v>
@@ -4676,10 +4676,10 @@
         <v>110</v>
       </c>
       <c r="B106" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C106" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>459</v>
@@ -4696,10 +4696,10 @@
         <v>111</v>
       </c>
       <c r="B107" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C107" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>460</v>
@@ -4716,10 +4716,10 @@
         <v>112</v>
       </c>
       <c r="B108" t="s">
-        <v>232</v>
+        <v>210</v>
       </c>
       <c r="C108" t="s">
-        <v>343</v>
+        <v>326</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>461</v>
@@ -4739,7 +4739,7 @@
         <v>233</v>
       </c>
       <c r="C109" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>462</v>
@@ -4759,7 +4759,7 @@
         <v>234</v>
       </c>
       <c r="C110" t="s">
-        <v>337</v>
+        <v>344</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>463</v>
@@ -4779,7 +4779,7 @@
         <v>235</v>
       </c>
       <c r="C111" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>464</v>
@@ -4799,7 +4799,7 @@
         <v>236</v>
       </c>
       <c r="C112" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>465</v>
@@ -4819,7 +4819,7 @@
         <v>237</v>
       </c>
       <c r="C113" t="s">
-        <v>322</v>
+        <v>345</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>466</v>
@@ -4839,7 +4839,7 @@
         <v>238</v>
       </c>
       <c r="C114" t="s">
-        <v>312</v>
+        <v>322</v>
       </c>
       <c r="D114" s="2" t="s">
         <v>467</v>
@@ -5019,7 +5019,7 @@
         <v>247</v>
       </c>
       <c r="C123" t="s">
-        <v>353</v>
+        <v>325</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>476</v>
@@ -5039,7 +5039,7 @@
         <v>248</v>
       </c>
       <c r="C124" t="s">
-        <v>325</v>
+        <v>353</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>477</v>

</xml_diff>